<commit_message>
Finished TE pathways, started TH pathways
</commit_message>
<xml_diff>
--- a/Pathway_analysis/consolidated_pathway_data.xlsx
+++ b/Pathway_analysis/consolidated_pathway_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="109">
   <si>
     <t>IMG_OID</t>
   </si>
@@ -345,6 +345,12 @@
   </si>
   <si>
     <t>Benzene degradation</t>
+  </si>
+  <si>
+    <t>GSB-Photosystem I reaction centers</t>
+  </si>
+  <si>
+    <t>GSB-Chlorosome</t>
   </si>
 </sst>
 </file>
@@ -360,15 +366,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -440,11 +452,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -455,6 +476,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,13 +794,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60D4974-3795-4306-8C06-8E8279D3D854}">
-  <dimension ref="A1:GN61"/>
+  <dimension ref="A1:GN63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="CU27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="EC33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="DA59" sqref="DA59"/>
+      <selection pane="bottomRight" activeCell="EH61" sqref="EH61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +822,19 @@
     <col min="105" max="105" width="11.85546875" style="1" customWidth="1"/>
     <col min="106" max="112" width="11.85546875" customWidth="1"/>
     <col min="113" max="113" width="11.85546875" style="1" customWidth="1"/>
-    <col min="114" max="196" width="11.85546875" customWidth="1"/>
+    <col min="114" max="115" width="11.85546875" customWidth="1"/>
+    <col min="116" max="116" width="11.85546875" style="1" customWidth="1"/>
+    <col min="117" max="117" width="11.85546875" customWidth="1"/>
+    <col min="118" max="118" width="11.85546875" style="1" customWidth="1"/>
+    <col min="119" max="130" width="11.85546875" customWidth="1"/>
+    <col min="131" max="131" width="11.85546875" style="11" customWidth="1"/>
+    <col min="132" max="132" width="11.85546875" customWidth="1"/>
+    <col min="133" max="133" width="11.85546875" style="11" customWidth="1"/>
+    <col min="134" max="136" width="11.85546875" customWidth="1"/>
+    <col min="137" max="137" width="11.85546875" style="11" customWidth="1"/>
+    <col min="138" max="144" width="11.85546875" customWidth="1"/>
+    <col min="145" max="145" width="11.85546875" style="11" customWidth="1"/>
+    <col min="146" max="196" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:196" x14ac:dyDescent="0.25">
@@ -1143,58 +1180,58 @@
       <c r="DK1">
         <v>2582580647</v>
       </c>
-      <c r="DL1">
+      <c r="DL1" s="1">
         <v>2582580622</v>
       </c>
       <c r="DM1">
         <v>2582580625</v>
       </c>
-      <c r="DN1">
+      <c r="DN1" s="5">
+        <v>2582580615</v>
+      </c>
+      <c r="DO1">
+        <v>2582580620</v>
+      </c>
+      <c r="DP1">
+        <v>2582580621</v>
+      </c>
+      <c r="DQ1">
+        <v>2582580623</v>
+      </c>
+      <c r="DR1">
+        <v>2582580624</v>
+      </c>
+      <c r="DS1">
+        <v>2582580629</v>
+      </c>
+      <c r="DT1">
+        <v>2582580633</v>
+      </c>
+      <c r="DU1">
+        <v>2582580637</v>
+      </c>
+      <c r="DV1">
+        <v>2582580639</v>
+      </c>
+      <c r="DW1">
+        <v>2582580642</v>
+      </c>
+      <c r="DX1">
+        <v>2582580644</v>
+      </c>
+      <c r="DY1">
+        <v>2582580646</v>
+      </c>
+      <c r="DZ1">
+        <v>2582580649</v>
+      </c>
+      <c r="EA1" s="5">
         <v>2582580650</v>
-      </c>
-      <c r="DO1">
-        <v>2582580629</v>
-      </c>
-      <c r="DP1">
-        <v>2582580644</v>
-      </c>
-      <c r="DQ1">
-        <v>2582580620</v>
-      </c>
-      <c r="DR1">
-        <v>2582580621</v>
-      </c>
-      <c r="DS1">
-        <v>2582580633</v>
-      </c>
-      <c r="DT1">
-        <v>2582580637</v>
-      </c>
-      <c r="DU1">
-        <v>2582580642</v>
-      </c>
-      <c r="DV1">
-        <v>2582580623</v>
-      </c>
-      <c r="DW1">
-        <v>2582580649</v>
-      </c>
-      <c r="DX1">
-        <v>2582580624</v>
-      </c>
-      <c r="DY1">
-        <v>2582580615</v>
-      </c>
-      <c r="DZ1">
-        <v>2582580639</v>
-      </c>
-      <c r="EA1">
-        <v>2582580646</v>
       </c>
       <c r="EB1">
         <v>2582580616</v>
       </c>
-      <c r="EC1">
+      <c r="EC1" s="11">
         <v>2582580638</v>
       </c>
       <c r="ED1">
@@ -1206,41 +1243,41 @@
       <c r="EF1">
         <v>2582580679</v>
       </c>
-      <c r="EG1">
+      <c r="EG1" s="11">
         <v>2582580706</v>
       </c>
       <c r="EH1">
+        <v>2582580657</v>
+      </c>
+      <c r="EI1">
+        <v>2582580670</v>
+      </c>
+      <c r="EJ1">
+        <v>2582580671</v>
+      </c>
+      <c r="EK1">
+        <v>2582580675</v>
+      </c>
+      <c r="EL1">
+        <v>2582580680</v>
+      </c>
+      <c r="EM1" s="3">
+        <v>2582580705</v>
+      </c>
+      <c r="EN1" s="12">
+        <v>2593339185</v>
+      </c>
+      <c r="EO1" s="11">
+        <v>2593339190</v>
+      </c>
+      <c r="EP1" s="13">
         <v>2582580662</v>
       </c>
-      <c r="EI1">
+      <c r="EQ1">
+        <v>2582580687</v>
+      </c>
+      <c r="ER1" s="13">
         <v>2582580672</v>
-      </c>
-      <c r="EJ1">
-        <v>2582580687</v>
-      </c>
-      <c r="EK1">
-        <v>2582580670</v>
-      </c>
-      <c r="EL1">
-        <v>2582580657</v>
-      </c>
-      <c r="EM1">
-        <v>2582580675</v>
-      </c>
-      <c r="EN1">
-        <v>2582580705</v>
-      </c>
-      <c r="EO1">
-        <v>2593339190</v>
-      </c>
-      <c r="EP1">
-        <v>2582580671</v>
-      </c>
-      <c r="EQ1">
-        <v>2593339185</v>
-      </c>
-      <c r="ER1">
-        <v>2582580680</v>
       </c>
       <c r="ES1">
         <v>2582580673</v>
@@ -1730,29 +1767,29 @@
       <c r="DK2" t="s">
         <v>10</v>
       </c>
-      <c r="DL2" t="s">
+      <c r="DL2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="DM2" t="s">
         <v>34</v>
       </c>
-      <c r="DN2" t="s">
-        <v>35</v>
+      <c r="DN2" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="DO2" t="s">
+        <v>18</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>18</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>19</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>37</v>
+      </c>
+      <c r="DS2" t="s">
         <v>36</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>18</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>18</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>18</v>
       </c>
       <c r="DT2" t="s">
         <v>18</v>
@@ -1761,27 +1798,27 @@
         <v>18</v>
       </c>
       <c r="DV2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="DW2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="DX2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="DY2" t="s">
         <v>22</v>
       </c>
       <c r="DZ2" t="s">
-        <v>22</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="EA2" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="EB2" t="s">
         <v>27</v>
       </c>
-      <c r="EC2" t="s">
+      <c r="EC2" s="11" t="s">
         <v>30</v>
       </c>
       <c r="ED2" t="s">
@@ -1793,41 +1830,41 @@
       <c r="EF2" t="s">
         <v>2</v>
       </c>
-      <c r="EG2" t="s">
+      <c r="EG2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="EH2" t="s">
+        <v>5</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>33</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>4</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>5</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>38</v>
+      </c>
+      <c r="EM2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="EN2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="EO2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="EP2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="EI2" t="s">
+      <c r="EQ2" t="s">
         <v>31</v>
       </c>
-      <c r="EJ2" t="s">
+      <c r="ER2" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>33</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>5</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>5</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>5</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>5</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>4</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>4</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>38</v>
       </c>
       <c r="ES2" t="s">
         <v>39</v>
@@ -2034,6 +2071,20 @@
         <v>73</v>
       </c>
       <c r="DI3" s="4"/>
+      <c r="DL3" s="4">
+        <v>82</v>
+      </c>
+      <c r="DM3" s="3">
+        <v>82</v>
+      </c>
+      <c r="DN3" s="4"/>
+      <c r="EA3" s="10"/>
+      <c r="EC3" s="10"/>
+      <c r="EG3" s="10"/>
+      <c r="EM3" s="3">
+        <v>73</v>
+      </c>
+      <c r="EO3" s="10"/>
     </row>
     <row r="4" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -2164,7 +2215,40 @@
       <c r="DG4" s="3">
         <v>60</v>
       </c>
-      <c r="DI4" s="4"/>
+      <c r="DI4" s="4">
+        <v>70</v>
+      </c>
+      <c r="DJ4" s="2">
+        <v>50</v>
+      </c>
+      <c r="DK4" s="2">
+        <v>90</v>
+      </c>
+      <c r="DL4" s="4">
+        <v>100</v>
+      </c>
+      <c r="DM4" s="2">
+        <v>100</v>
+      </c>
+      <c r="DN4" s="4"/>
+      <c r="DU4" s="3">
+        <v>70</v>
+      </c>
+      <c r="EA4" s="10"/>
+      <c r="EC4" s="10">
+        <v>70</v>
+      </c>
+      <c r="EG4" s="10"/>
+      <c r="EL4" s="3">
+        <v>60</v>
+      </c>
+      <c r="EM4" s="3">
+        <v>80</v>
+      </c>
+      <c r="EN4" s="3">
+        <v>70</v>
+      </c>
+      <c r="EO4" s="10"/>
     </row>
     <row r="5" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -2199,6 +2283,20 @@
       <c r="CY5" s="4"/>
       <c r="DA5" s="4"/>
       <c r="DI5" s="4"/>
+      <c r="DL5" s="4"/>
+      <c r="DN5" s="4">
+        <v>100</v>
+      </c>
+      <c r="DV5" s="3">
+        <v>100</v>
+      </c>
+      <c r="DY5" s="3">
+        <v>100</v>
+      </c>
+      <c r="EA5" s="10"/>
+      <c r="EC5" s="10"/>
+      <c r="EG5" s="10"/>
+      <c r="EO5" s="10"/>
     </row>
     <row r="6" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
@@ -2233,6 +2331,12 @@
       <c r="CY6" s="4"/>
       <c r="DA6" s="4"/>
       <c r="DI6" s="4"/>
+      <c r="DL6" s="4"/>
+      <c r="DN6" s="4"/>
+      <c r="EA6" s="10"/>
+      <c r="EC6" s="10"/>
+      <c r="EG6" s="10"/>
+      <c r="EO6" s="10"/>
     </row>
     <row r="7" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -2537,7 +2641,99 @@
       <c r="DH7" s="2">
         <v>50</v>
       </c>
-      <c r="DI7" s="4"/>
+      <c r="DI7" s="4">
+        <v>50</v>
+      </c>
+      <c r="DK7" s="2">
+        <v>50</v>
+      </c>
+      <c r="DL7" s="4">
+        <v>50</v>
+      </c>
+      <c r="DM7" s="2">
+        <v>50</v>
+      </c>
+      <c r="DN7" s="4">
+        <v>80</v>
+      </c>
+      <c r="DO7" s="2">
+        <v>50</v>
+      </c>
+      <c r="DQ7" s="2">
+        <v>100</v>
+      </c>
+      <c r="DR7" s="2">
+        <v>50</v>
+      </c>
+      <c r="DS7" s="2">
+        <v>50</v>
+      </c>
+      <c r="DT7" s="2">
+        <v>50</v>
+      </c>
+      <c r="DU7" s="2">
+        <v>100</v>
+      </c>
+      <c r="DV7" s="2">
+        <v>100</v>
+      </c>
+      <c r="DW7" s="2">
+        <v>50</v>
+      </c>
+      <c r="DX7" s="2">
+        <v>50</v>
+      </c>
+      <c r="DY7" s="2">
+        <v>60</v>
+      </c>
+      <c r="DZ7" s="2">
+        <v>100</v>
+      </c>
+      <c r="EA7" s="10">
+        <v>100</v>
+      </c>
+      <c r="EB7" s="2">
+        <v>50</v>
+      </c>
+      <c r="EC7" s="10">
+        <v>100</v>
+      </c>
+      <c r="ED7" s="2">
+        <v>50</v>
+      </c>
+      <c r="EE7" s="2">
+        <v>50</v>
+      </c>
+      <c r="EF7" s="2">
+        <v>50</v>
+      </c>
+      <c r="EG7" s="10">
+        <v>50</v>
+      </c>
+      <c r="EH7" s="2">
+        <v>50</v>
+      </c>
+      <c r="EI7" s="2">
+        <v>50</v>
+      </c>
+      <c r="EJ7" s="2">
+        <v>50</v>
+      </c>
+      <c r="EK7" s="2">
+        <v>50</v>
+      </c>
+      <c r="EL7" s="2">
+        <v>50</v>
+      </c>
+      <c r="EM7" s="2">
+        <v>100</v>
+      </c>
+      <c r="EN7" s="2">
+        <v>50</v>
+      </c>
+      <c r="EO7" s="10">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
@@ -2605,6 +2801,12 @@
       <c r="CZ8" s="2"/>
       <c r="DA8" s="4"/>
       <c r="DI8" s="4"/>
+      <c r="DL8" s="4"/>
+      <c r="DN8" s="4"/>
+      <c r="EA8" s="10"/>
+      <c r="EC8" s="10"/>
+      <c r="EG8" s="10"/>
+      <c r="EO8" s="10"/>
     </row>
     <row r="9" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -2700,6 +2902,45 @@
         <v>100</v>
       </c>
       <c r="DI9" s="4"/>
+      <c r="DK9" s="3">
+        <v>100</v>
+      </c>
+      <c r="DL9" s="4"/>
+      <c r="DN9" s="4">
+        <v>100</v>
+      </c>
+      <c r="DO9" s="3">
+        <v>100</v>
+      </c>
+      <c r="DP9" s="2">
+        <v>100</v>
+      </c>
+      <c r="DQ9" s="2">
+        <v>100</v>
+      </c>
+      <c r="DT9" s="3">
+        <v>100</v>
+      </c>
+      <c r="DU9" s="3">
+        <v>100</v>
+      </c>
+      <c r="DV9" s="3">
+        <v>100</v>
+      </c>
+      <c r="DW9" s="3">
+        <v>100</v>
+      </c>
+      <c r="DZ9" s="3">
+        <v>100</v>
+      </c>
+      <c r="EA9" s="10"/>
+      <c r="EC9" s="10">
+        <v>100</v>
+      </c>
+      <c r="EG9" s="10">
+        <v>100</v>
+      </c>
+      <c r="EO9" s="10"/>
     </row>
     <row r="10" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
@@ -2744,7 +2985,16 @@
       <c r="CQ10" s="4"/>
       <c r="CY10" s="4"/>
       <c r="DA10" s="4"/>
-      <c r="DI10" s="4"/>
+      <c r="DN10" s="4"/>
+      <c r="DV10" s="3">
+        <v>56</v>
+      </c>
+      <c r="EA10" s="10"/>
+      <c r="EC10" s="10">
+        <v>56</v>
+      </c>
+      <c r="EG10" s="10"/>
+      <c r="EO10" s="10"/>
     </row>
     <row r="11" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
@@ -2881,7 +3131,42 @@
       <c r="DH11" s="3">
         <v>100</v>
       </c>
-      <c r="DI11" s="4"/>
+      <c r="DI11" s="4">
+        <v>67</v>
+      </c>
+      <c r="DL11" s="4">
+        <v>67</v>
+      </c>
+      <c r="DM11" s="3">
+        <v>67</v>
+      </c>
+      <c r="DN11" s="4"/>
+      <c r="DU11" s="3">
+        <v>67</v>
+      </c>
+      <c r="DV11" s="3">
+        <v>67</v>
+      </c>
+      <c r="DY11" s="3">
+        <v>67</v>
+      </c>
+      <c r="EA11" s="10"/>
+      <c r="EC11" s="10">
+        <v>100</v>
+      </c>
+      <c r="EG11" s="10"/>
+      <c r="EH11" s="3">
+        <v>67</v>
+      </c>
+      <c r="EL11" s="3">
+        <v>67</v>
+      </c>
+      <c r="EM11" s="3">
+        <v>67</v>
+      </c>
+      <c r="EO11" s="10">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
@@ -2938,6 +3223,35 @@
       <c r="CY12" s="4"/>
       <c r="DA12" s="4"/>
       <c r="DI12" s="4"/>
+      <c r="DL12" s="4">
+        <v>50</v>
+      </c>
+      <c r="DM12" s="3">
+        <v>50</v>
+      </c>
+      <c r="DN12" s="4"/>
+      <c r="DO12" s="3">
+        <v>50</v>
+      </c>
+      <c r="DP12" s="2">
+        <v>50</v>
+      </c>
+      <c r="DT12" s="3">
+        <v>50</v>
+      </c>
+      <c r="DV12" s="3">
+        <v>50</v>
+      </c>
+      <c r="DW12" s="3">
+        <v>50</v>
+      </c>
+      <c r="EA12" s="10"/>
+      <c r="EC12" s="10"/>
+      <c r="EG12" s="10"/>
+      <c r="EL12" s="3">
+        <v>100</v>
+      </c>
+      <c r="EO12" s="10"/>
     </row>
     <row r="13" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
@@ -3000,6 +3314,23 @@
       </c>
       <c r="DA13" s="4"/>
       <c r="DI13" s="4"/>
+      <c r="DL13" s="4">
+        <v>100</v>
+      </c>
+      <c r="DM13" s="3">
+        <v>100</v>
+      </c>
+      <c r="DN13" s="4"/>
+      <c r="DT13" s="3">
+        <v>100</v>
+      </c>
+      <c r="DY13" s="3">
+        <v>50</v>
+      </c>
+      <c r="EA13" s="10"/>
+      <c r="EC13" s="10"/>
+      <c r="EG13" s="10"/>
+      <c r="EO13" s="10"/>
     </row>
     <row r="14" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
@@ -3056,6 +3387,19 @@
       </c>
       <c r="DA14" s="4"/>
       <c r="DI14" s="4"/>
+      <c r="DL14" s="4"/>
+      <c r="DN14" s="4">
+        <v>50</v>
+      </c>
+      <c r="DO14" s="3">
+        <v>50</v>
+      </c>
+      <c r="EA14" s="10"/>
+      <c r="EC14" s="10">
+        <v>100</v>
+      </c>
+      <c r="EG14" s="10"/>
+      <c r="EO14" s="10"/>
     </row>
     <row r="15" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
@@ -3115,6 +3459,15 @@
       </c>
       <c r="DA15" s="4"/>
       <c r="DI15" s="4"/>
+      <c r="DL15" s="4"/>
+      <c r="DN15" s="4"/>
+      <c r="DO15" s="3">
+        <v>50</v>
+      </c>
+      <c r="EA15" s="10"/>
+      <c r="EC15" s="10"/>
+      <c r="EG15" s="10"/>
+      <c r="EO15" s="10"/>
     </row>
     <row r="16" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
@@ -3135,8 +3488,20 @@
       <c r="CY16" s="4"/>
       <c r="DA16" s="4"/>
       <c r="DI16" s="4"/>
+      <c r="DL16" s="4"/>
+      <c r="DN16" s="4"/>
+      <c r="DU16" s="3">
+        <v>50</v>
+      </c>
+      <c r="DV16" s="3">
+        <v>50</v>
+      </c>
+      <c r="EA16" s="10"/>
+      <c r="EC16" s="10"/>
+      <c r="EG16" s="10"/>
+      <c r="EO16" s="10"/>
     </row>
-    <row r="17" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>53</v>
       </c>
@@ -3252,8 +3617,31 @@
       </c>
       <c r="DA17" s="4"/>
       <c r="DI17" s="4"/>
+      <c r="DL17" s="4"/>
+      <c r="DN17" s="4">
+        <v>100</v>
+      </c>
+      <c r="DO17" s="3">
+        <v>100</v>
+      </c>
+      <c r="DR17" s="3">
+        <v>100</v>
+      </c>
+      <c r="DT17" s="3">
+        <v>100</v>
+      </c>
+      <c r="DW17" s="3">
+        <v>100</v>
+      </c>
+      <c r="EA17" s="10"/>
+      <c r="EC17" s="10"/>
+      <c r="EG17" s="10"/>
+      <c r="EL17" s="3">
+        <v>100</v>
+      </c>
+      <c r="EO17" s="10"/>
     </row>
-    <row r="18" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>54</v>
       </c>
@@ -3316,8 +3704,18 @@
         <v>100</v>
       </c>
       <c r="DI18" s="4"/>
+      <c r="DL18" s="4"/>
+      <c r="DN18" s="4">
+        <v>100</v>
+      </c>
+      <c r="EA18" s="10"/>
+      <c r="EC18" s="10">
+        <v>100</v>
+      </c>
+      <c r="EG18" s="10"/>
+      <c r="EO18" s="10"/>
     </row>
-    <row r="19" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>79</v>
       </c>
@@ -3389,8 +3787,38 @@
       <c r="CY19" s="4"/>
       <c r="DA19" s="4"/>
       <c r="DI19" s="4"/>
+      <c r="DL19" s="4">
+        <v>100</v>
+      </c>
+      <c r="DM19" s="3">
+        <v>100</v>
+      </c>
+      <c r="DN19" s="4">
+        <v>100</v>
+      </c>
+      <c r="DP19" s="2">
+        <v>100</v>
+      </c>
+      <c r="DQ19" s="2">
+        <v>100</v>
+      </c>
+      <c r="DU19" s="3">
+        <v>100</v>
+      </c>
+      <c r="DV19" s="3">
+        <v>100</v>
+      </c>
+      <c r="EA19" s="10"/>
+      <c r="EC19" s="10">
+        <v>100</v>
+      </c>
+      <c r="EG19" s="10"/>
+      <c r="EJ19" s="3">
+        <v>100</v>
+      </c>
+      <c r="EO19" s="10"/>
     </row>
-    <row r="20" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>82</v>
       </c>
@@ -3561,8 +3989,53 @@
         <v>67</v>
       </c>
       <c r="DI20" s="4"/>
+      <c r="DL20" s="4">
+        <v>67</v>
+      </c>
+      <c r="DM20" s="3">
+        <v>67</v>
+      </c>
+      <c r="DN20" s="4">
+        <v>100</v>
+      </c>
+      <c r="DP20" s="2">
+        <v>100</v>
+      </c>
+      <c r="DQ20" s="2">
+        <v>100</v>
+      </c>
+      <c r="DT20" s="3">
+        <v>100</v>
+      </c>
+      <c r="DU20" s="3">
+        <v>100</v>
+      </c>
+      <c r="DV20" s="3">
+        <v>100</v>
+      </c>
+      <c r="DY20" s="3">
+        <v>100</v>
+      </c>
+      <c r="EA20" s="10"/>
+      <c r="EB20" s="3">
+        <v>100</v>
+      </c>
+      <c r="EC20" s="10">
+        <v>100</v>
+      </c>
+      <c r="EG20" s="10"/>
+      <c r="EI20" s="3">
+        <v>67</v>
+      </c>
+      <c r="EJ20" s="3">
+        <v>67</v>
+      </c>
+      <c r="EN20" s="3">
+        <v>67</v>
+      </c>
+      <c r="EO20" s="10"/>
     </row>
-    <row r="21" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>81</v>
       </c>
@@ -3585,8 +4058,19 @@
       <c r="CY21" s="4"/>
       <c r="DA21" s="4"/>
       <c r="DI21" s="4"/>
+      <c r="DL21" s="4">
+        <v>67</v>
+      </c>
+      <c r="DM21" s="3">
+        <v>67</v>
+      </c>
+      <c r="DN21" s="4"/>
+      <c r="EA21" s="10"/>
+      <c r="EC21" s="10"/>
+      <c r="EG21" s="10"/>
+      <c r="EO21" s="10"/>
     </row>
-    <row r="22" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>70</v>
       </c>
@@ -3618,8 +4102,32 @@
       <c r="CY22" s="4"/>
       <c r="DA22" s="4"/>
       <c r="DI22" s="4"/>
+      <c r="DL22" s="4"/>
+      <c r="DN22" s="4"/>
+      <c r="DO22" s="3">
+        <v>100</v>
+      </c>
+      <c r="DP22" s="3">
+        <v>100</v>
+      </c>
+      <c r="DQ22" s="3">
+        <v>100</v>
+      </c>
+      <c r="DT22" s="3">
+        <v>100</v>
+      </c>
+      <c r="DW22" s="3">
+        <v>100</v>
+      </c>
+      <c r="DZ22" s="3">
+        <v>100</v>
+      </c>
+      <c r="EA22" s="10"/>
+      <c r="EC22" s="10"/>
+      <c r="EG22" s="10"/>
+      <c r="EO22" s="10"/>
     </row>
-    <row r="23" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>80</v>
       </c>
@@ -3899,9 +4407,87 @@
       <c r="DH23" s="3">
         <v>100</v>
       </c>
-      <c r="DI23" s="4"/>
+      <c r="DI23" s="4">
+        <v>100</v>
+      </c>
+      <c r="DJ23" s="2">
+        <v>100</v>
+      </c>
+      <c r="DK23" s="2">
+        <v>100</v>
+      </c>
+      <c r="DL23" s="4">
+        <v>100</v>
+      </c>
+      <c r="DM23" s="2">
+        <v>100</v>
+      </c>
+      <c r="DN23" s="4">
+        <v>100</v>
+      </c>
+      <c r="DP23" s="2">
+        <v>100</v>
+      </c>
+      <c r="DQ23" s="2">
+        <v>100</v>
+      </c>
+      <c r="DR23" s="2">
+        <v>100</v>
+      </c>
+      <c r="DT23" s="3">
+        <v>100</v>
+      </c>
+      <c r="DU23" s="3">
+        <v>100</v>
+      </c>
+      <c r="DV23" s="3">
+        <v>100</v>
+      </c>
+      <c r="DW23" s="3">
+        <v>100</v>
+      </c>
+      <c r="DX23" s="3">
+        <v>100</v>
+      </c>
+      <c r="DY23" s="3">
+        <v>100</v>
+      </c>
+      <c r="DZ23" s="3">
+        <v>100</v>
+      </c>
+      <c r="EA23" s="10">
+        <v>100</v>
+      </c>
+      <c r="EB23" s="2">
+        <v>100</v>
+      </c>
+      <c r="EC23" s="10">
+        <v>100</v>
+      </c>
+      <c r="EG23" s="10"/>
+      <c r="EI23" s="3">
+        <v>100</v>
+      </c>
+      <c r="EJ23" s="3">
+        <v>100</v>
+      </c>
+      <c r="EK23" s="3">
+        <v>100</v>
+      </c>
+      <c r="EL23" s="2">
+        <v>100</v>
+      </c>
+      <c r="EM23" s="2">
+        <v>100</v>
+      </c>
+      <c r="EN23" s="2">
+        <v>100</v>
+      </c>
+      <c r="EO23" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="24" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>68</v>
       </c>
@@ -4185,9 +4771,72 @@
       <c r="DH24" s="2">
         <v>100</v>
       </c>
-      <c r="DI24" s="4"/>
+      <c r="DI24" s="4">
+        <v>100</v>
+      </c>
+      <c r="DK24" s="2">
+        <v>100</v>
+      </c>
+      <c r="DL24" s="4">
+        <v>100</v>
+      </c>
+      <c r="DM24" s="2">
+        <v>100</v>
+      </c>
+      <c r="DN24" s="4">
+        <v>100</v>
+      </c>
+      <c r="DQ24" s="2">
+        <v>100</v>
+      </c>
+      <c r="DU24" s="3">
+        <v>100</v>
+      </c>
+      <c r="DV24" s="3">
+        <v>100</v>
+      </c>
+      <c r="DY24" s="3">
+        <v>100</v>
+      </c>
+      <c r="DZ24" s="3">
+        <v>100</v>
+      </c>
+      <c r="EA24" s="10">
+        <v>100</v>
+      </c>
+      <c r="EB24" s="2">
+        <v>100</v>
+      </c>
+      <c r="EC24" s="10">
+        <v>100</v>
+      </c>
+      <c r="EG24" s="10"/>
+      <c r="EH24" s="3">
+        <v>100</v>
+      </c>
+      <c r="EI24" s="3">
+        <v>100</v>
+      </c>
+      <c r="EJ24" s="3">
+        <v>100</v>
+      </c>
+      <c r="EK24" s="2">
+        <v>100</v>
+      </c>
+      <c r="EL24" s="2">
+        <v>100</v>
+      </c>
+      <c r="EM24" s="2">
+        <v>100</v>
+      </c>
+      <c r="EN24" s="2">
+        <v>100</v>
+      </c>
+      <c r="EO24" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="25" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
@@ -4504,9 +5153,96 @@
       <c r="DH25" s="2">
         <v>63</v>
       </c>
-      <c r="DI25" s="4"/>
+      <c r="DI25" s="4">
+        <v>88</v>
+      </c>
+      <c r="DJ25" s="2">
+        <v>63</v>
+      </c>
+      <c r="DK25" s="2">
+        <v>100</v>
+      </c>
+      <c r="DL25" s="4">
+        <v>100</v>
+      </c>
+      <c r="DM25" s="2">
+        <v>100</v>
+      </c>
+      <c r="DN25" s="4">
+        <v>88</v>
+      </c>
+      <c r="DO25" s="2">
+        <v>100</v>
+      </c>
+      <c r="DP25" s="2">
+        <v>63</v>
+      </c>
+      <c r="DQ25" s="2">
+        <v>88</v>
+      </c>
+      <c r="DR25" s="2">
+        <v>63</v>
+      </c>
+      <c r="DS25" s="2">
+        <v>100</v>
+      </c>
+      <c r="DT25" s="2">
+        <v>100</v>
+      </c>
+      <c r="DU25" s="2">
+        <v>75</v>
+      </c>
+      <c r="DV25" s="2">
+        <v>88</v>
+      </c>
+      <c r="DW25" s="2">
+        <v>100</v>
+      </c>
+      <c r="DX25" s="2">
+        <v>100</v>
+      </c>
+      <c r="DY25" s="2">
+        <v>63</v>
+      </c>
+      <c r="DZ25" s="2">
+        <v>63</v>
+      </c>
+      <c r="EA25" s="10">
+        <v>100</v>
+      </c>
+      <c r="EB25" s="2">
+        <v>100</v>
+      </c>
+      <c r="EC25" s="10">
+        <v>88</v>
+      </c>
+      <c r="EG25" s="10"/>
+      <c r="EH25" s="3">
+        <v>75</v>
+      </c>
+      <c r="EI25" s="3">
+        <v>88</v>
+      </c>
+      <c r="EJ25" s="3">
+        <v>100</v>
+      </c>
+      <c r="EK25" s="2">
+        <v>75</v>
+      </c>
+      <c r="EL25" s="2">
+        <v>63</v>
+      </c>
+      <c r="EM25" s="2">
+        <v>100</v>
+      </c>
+      <c r="EN25" s="2">
+        <v>100</v>
+      </c>
+      <c r="EO25" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="26" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>56</v>
       </c>
@@ -4698,9 +5434,70 @@
       <c r="DH26" s="2">
         <v>100</v>
       </c>
-      <c r="DI26" s="4"/>
+      <c r="DI26" s="4">
+        <v>50</v>
+      </c>
+      <c r="DL26" s="4">
+        <v>100</v>
+      </c>
+      <c r="DM26" s="2">
+        <v>100</v>
+      </c>
+      <c r="DN26" s="4">
+        <v>100</v>
+      </c>
+      <c r="DP26" s="2"/>
+      <c r="DQ26" s="2">
+        <v>100</v>
+      </c>
+      <c r="DR26" s="2"/>
+      <c r="DS26" s="2"/>
+      <c r="DT26" s="2">
+        <v>50</v>
+      </c>
+      <c r="DU26" s="2">
+        <v>50</v>
+      </c>
+      <c r="DV26" s="2">
+        <v>100</v>
+      </c>
+      <c r="DW26" s="2"/>
+      <c r="DX26" s="2"/>
+      <c r="DY26" s="2">
+        <v>100</v>
+      </c>
+      <c r="DZ26" s="2">
+        <v>100</v>
+      </c>
+      <c r="EA26" s="10"/>
+      <c r="EC26" s="10">
+        <v>100</v>
+      </c>
+      <c r="EE26" s="3">
+        <v>50</v>
+      </c>
+      <c r="EG26" s="10"/>
+      <c r="EH26" s="3">
+        <v>100</v>
+      </c>
+      <c r="EJ26" s="2"/>
+      <c r="EK26" s="2">
+        <v>100</v>
+      </c>
+      <c r="EL26" s="2">
+        <v>100</v>
+      </c>
+      <c r="EM26" s="2">
+        <v>100</v>
+      </c>
+      <c r="EN26" s="2">
+        <v>100</v>
+      </c>
+      <c r="EO26" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="27" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>57</v>
       </c>
@@ -5014,9 +5811,100 @@
       <c r="DH27" s="2">
         <v>100</v>
       </c>
-      <c r="DI27" s="4"/>
+      <c r="DI27" s="4">
+        <v>50</v>
+      </c>
+      <c r="DJ27" s="2">
+        <v>75</v>
+      </c>
+      <c r="DK27" s="2">
+        <v>100</v>
+      </c>
+      <c r="DL27" s="4">
+        <v>100</v>
+      </c>
+      <c r="DM27" s="2">
+        <v>100</v>
+      </c>
+      <c r="DN27" s="4">
+        <v>50</v>
+      </c>
+      <c r="DO27" s="2">
+        <v>50</v>
+      </c>
+      <c r="DP27" s="2">
+        <v>100</v>
+      </c>
+      <c r="DQ27" s="2">
+        <v>100</v>
+      </c>
+      <c r="DR27" s="2">
+        <v>75</v>
+      </c>
+      <c r="DS27" s="2">
+        <v>100</v>
+      </c>
+      <c r="DT27" s="2">
+        <v>100</v>
+      </c>
+      <c r="DU27" s="2">
+        <v>100</v>
+      </c>
+      <c r="DV27" s="2">
+        <v>100</v>
+      </c>
+      <c r="DW27" s="2">
+        <v>75</v>
+      </c>
+      <c r="DX27" s="2">
+        <v>100</v>
+      </c>
+      <c r="DY27" s="2">
+        <v>75</v>
+      </c>
+      <c r="DZ27" s="2">
+        <v>100</v>
+      </c>
+      <c r="EA27" s="10">
+        <v>100</v>
+      </c>
+      <c r="EB27" s="2">
+        <v>75</v>
+      </c>
+      <c r="EC27" s="10">
+        <v>100</v>
+      </c>
+      <c r="ED27" s="2">
+        <v>75</v>
+      </c>
+      <c r="EF27" s="2">
+        <v>50</v>
+      </c>
+      <c r="EG27" s="10"/>
+      <c r="EH27" s="3">
+        <v>75</v>
+      </c>
+      <c r="EI27" s="3">
+        <v>75</v>
+      </c>
+      <c r="EJ27" s="3">
+        <v>75</v>
+      </c>
+      <c r="EK27" s="2">
+        <v>100</v>
+      </c>
+      <c r="EL27" s="2">
+        <v>75</v>
+      </c>
+      <c r="EM27" s="2">
+        <v>100</v>
+      </c>
+      <c r="EN27" s="2">
+        <v>100</v>
+      </c>
+      <c r="EO27" s="10"/>
     </row>
-    <row r="28" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>95</v>
       </c>
@@ -5060,8 +5948,29 @@
       <c r="CY28" s="4"/>
       <c r="DA28" s="4"/>
       <c r="DI28" s="4"/>
+      <c r="DL28" s="4"/>
+      <c r="DM28" s="2"/>
+      <c r="DN28" s="4">
+        <v>100</v>
+      </c>
+      <c r="DU28" s="2">
+        <v>75</v>
+      </c>
+      <c r="DV28" s="2">
+        <v>100</v>
+      </c>
+      <c r="DY28" s="2">
+        <v>100</v>
+      </c>
+      <c r="DZ28" s="2">
+        <v>100</v>
+      </c>
+      <c r="EA28" s="10"/>
+      <c r="EC28" s="10"/>
+      <c r="EG28" s="10"/>
+      <c r="EO28" s="10"/>
     </row>
-    <row r="29" spans="2:113" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:145" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
         <v>96</v>
       </c>
@@ -5168,8 +6077,22 @@
         <v>50</v>
       </c>
       <c r="DI29" s="4"/>
+      <c r="DL29" s="4"/>
+      <c r="DN29" s="4"/>
+      <c r="EA29" s="10"/>
+      <c r="EB29" s="3">
+        <v>50</v>
+      </c>
+      <c r="EC29" s="10">
+        <v>50</v>
+      </c>
+      <c r="EG29" s="10"/>
+      <c r="EK29" s="3">
+        <v>100</v>
+      </c>
+      <c r="EO29" s="10"/>
     </row>
-    <row r="30" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>83</v>
       </c>
@@ -5248,8 +6171,23 @@
       <c r="CY30" s="4"/>
       <c r="DA30" s="4"/>
       <c r="DI30" s="4"/>
+      <c r="DL30" s="4"/>
+      <c r="DN30" s="4"/>
+      <c r="DU30" s="3">
+        <v>50</v>
+      </c>
+      <c r="EA30" s="10"/>
+      <c r="EB30" s="3">
+        <v>75</v>
+      </c>
+      <c r="EC30" s="10"/>
+      <c r="EG30" s="10"/>
+      <c r="EL30" s="3">
+        <v>50</v>
+      </c>
+      <c r="EO30" s="10"/>
     </row>
-    <row r="31" spans="2:113" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:145" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>84</v>
       </c>
@@ -5285,8 +6223,16 @@
         <v>100</v>
       </c>
       <c r="DI31" s="4"/>
+      <c r="DL31" s="4"/>
+      <c r="DN31" s="4"/>
+      <c r="EA31" s="10"/>
+      <c r="EC31" s="10">
+        <v>67</v>
+      </c>
+      <c r="EG31" s="10"/>
+      <c r="EO31" s="10"/>
     </row>
-    <row r="32" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>85</v>
       </c>
@@ -5441,8 +6387,39 @@
         <v>50</v>
       </c>
       <c r="DI32" s="4"/>
+      <c r="DL32" s="4"/>
+      <c r="DN32" s="4"/>
+      <c r="DU32" s="3">
+        <v>50</v>
+      </c>
+      <c r="EA32" s="10"/>
+      <c r="EB32" s="3">
+        <v>100</v>
+      </c>
+      <c r="EC32" s="10">
+        <v>100</v>
+      </c>
+      <c r="EG32" s="10"/>
+      <c r="EH32" s="3">
+        <v>50</v>
+      </c>
+      <c r="EJ32" s="3">
+        <v>50</v>
+      </c>
+      <c r="EK32" s="3">
+        <v>100</v>
+      </c>
+      <c r="EL32" s="2">
+        <v>50</v>
+      </c>
+      <c r="EM32" s="2">
+        <v>100</v>
+      </c>
+      <c r="EO32" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="33" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>86</v>
       </c>
@@ -5674,9 +6651,73 @@
       <c r="DH33" s="3">
         <v>100</v>
       </c>
-      <c r="DI33" s="4"/>
+      <c r="DI33" s="4">
+        <v>100</v>
+      </c>
+      <c r="DK33" s="2">
+        <v>50</v>
+      </c>
+      <c r="DL33" s="4">
+        <v>50</v>
+      </c>
+      <c r="DM33" s="2">
+        <v>100</v>
+      </c>
+      <c r="DN33" s="4">
+        <v>100</v>
+      </c>
+      <c r="DP33" s="2">
+        <v>50</v>
+      </c>
+      <c r="DU33" s="3">
+        <v>100</v>
+      </c>
+      <c r="DV33" s="3">
+        <v>100</v>
+      </c>
+      <c r="DW33" s="3">
+        <v>50</v>
+      </c>
+      <c r="DY33" s="3">
+        <v>100</v>
+      </c>
+      <c r="EA33" s="10"/>
+      <c r="EC33" s="10">
+        <v>100</v>
+      </c>
+      <c r="ED33" s="3">
+        <v>50</v>
+      </c>
+      <c r="EF33" s="3">
+        <v>50</v>
+      </c>
+      <c r="EG33" s="10"/>
+      <c r="EH33" s="2">
+        <v>100</v>
+      </c>
+      <c r="EI33" s="2">
+        <v>100</v>
+      </c>
+      <c r="EJ33" s="2">
+        <v>100</v>
+      </c>
+      <c r="EK33" s="2">
+        <v>100</v>
+      </c>
+      <c r="EL33" s="2">
+        <v>100</v>
+      </c>
+      <c r="EM33" s="2">
+        <v>100</v>
+      </c>
+      <c r="EN33" s="2">
+        <v>100</v>
+      </c>
+      <c r="EO33" s="10">
+        <v>100</v>
+      </c>
     </row>
-    <row r="34" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>87</v>
       </c>
@@ -5745,9 +6786,22 @@
       <c r="DH34" s="3">
         <v>80</v>
       </c>
-      <c r="DI34" s="4"/>
+      <c r="DI34" s="4">
+        <v>100</v>
+      </c>
+      <c r="DJ34" s="3">
+        <v>100</v>
+      </c>
+      <c r="DL34" s="4"/>
+      <c r="DN34" s="4"/>
+      <c r="EA34" s="10"/>
+      <c r="EC34" s="10">
+        <v>80</v>
+      </c>
+      <c r="EG34" s="10"/>
+      <c r="EO34" s="10"/>
     </row>
-    <row r="35" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>100</v>
       </c>
@@ -5863,9 +6917,34 @@
       <c r="DG35" s="2">
         <v>75</v>
       </c>
-      <c r="DI35" s="4"/>
+      <c r="DI35" s="4">
+        <v>50</v>
+      </c>
+      <c r="DL35" s="4"/>
+      <c r="DN35" s="4"/>
+      <c r="DU35" s="3">
+        <v>71</v>
+      </c>
+      <c r="EA35" s="10"/>
+      <c r="EB35" s="3">
+        <v>50</v>
+      </c>
+      <c r="EC35" s="10">
+        <v>75</v>
+      </c>
+      <c r="EG35" s="10"/>
+      <c r="EK35" s="3">
+        <v>75</v>
+      </c>
+      <c r="EM35" s="3">
+        <v>100</v>
+      </c>
+      <c r="EN35" s="3">
+        <v>75</v>
+      </c>
+      <c r="EO35" s="10"/>
     </row>
-    <row r="36" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>101</v>
       </c>
@@ -5955,8 +7034,22 @@
         <v>80</v>
       </c>
       <c r="DI36" s="4"/>
+      <c r="DL36" s="4"/>
+      <c r="DN36" s="4">
+        <v>100</v>
+      </c>
+      <c r="DV36" s="3">
+        <v>100</v>
+      </c>
+      <c r="DY36" s="3">
+        <v>60</v>
+      </c>
+      <c r="EA36" s="10"/>
+      <c r="EC36" s="10"/>
+      <c r="EG36" s="10"/>
+      <c r="EO36" s="10"/>
     </row>
-    <row r="37" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>88</v>
       </c>
@@ -6011,8 +7104,31 @@
       </c>
       <c r="DA37" s="4"/>
       <c r="DI37" s="4"/>
+      <c r="DL37" s="4"/>
+      <c r="DN37" s="4"/>
+      <c r="DO37" s="3">
+        <v>100</v>
+      </c>
+      <c r="DP37" s="3">
+        <v>60</v>
+      </c>
+      <c r="DT37" s="3">
+        <v>100</v>
+      </c>
+      <c r="DU37" s="3">
+        <v>60</v>
+      </c>
+      <c r="DW37" s="3">
+        <v>100</v>
+      </c>
+      <c r="EA37" s="10">
+        <v>80</v>
+      </c>
+      <c r="EC37" s="10"/>
+      <c r="EG37" s="10"/>
+      <c r="EO37" s="10"/>
     </row>
-    <row r="38" spans="2:113" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:145" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>58</v>
       </c>
@@ -6105,8 +7221,33 @@
         <v>67</v>
       </c>
       <c r="DI38" s="4"/>
+      <c r="DL38" s="4"/>
+      <c r="DN38" s="4"/>
+      <c r="DO38" s="3">
+        <v>100</v>
+      </c>
+      <c r="DP38" s="3">
+        <v>100</v>
+      </c>
+      <c r="DT38" s="3">
+        <v>100</v>
+      </c>
+      <c r="DU38" s="3">
+        <v>100</v>
+      </c>
+      <c r="DW38" s="3">
+        <v>100</v>
+      </c>
+      <c r="EA38" s="10">
+        <v>100</v>
+      </c>
+      <c r="EC38" s="10">
+        <v>100</v>
+      </c>
+      <c r="EG38" s="10"/>
+      <c r="EO38" s="10"/>
     </row>
-    <row r="39" spans="2:113" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:145" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>59</v>
       </c>
@@ -6238,8 +7379,44 @@
       <c r="DH39">
         <v>60</v>
       </c>
+      <c r="DI39" s="1">
+        <v>60</v>
+      </c>
+      <c r="DL39" s="1">
+        <v>60</v>
+      </c>
+      <c r="DM39" s="2">
+        <v>60</v>
+      </c>
+      <c r="DU39" s="3">
+        <v>60</v>
+      </c>
+      <c r="EA39" s="11">
+        <v>60</v>
+      </c>
+      <c r="EB39">
+        <v>60</v>
+      </c>
+      <c r="EC39" s="11">
+        <v>60</v>
+      </c>
+      <c r="EH39">
+        <v>60</v>
+      </c>
+      <c r="EK39">
+        <v>60</v>
+      </c>
+      <c r="EL39">
+        <v>60</v>
+      </c>
+      <c r="EN39">
+        <v>60</v>
+      </c>
+      <c r="EO39" s="11">
+        <v>60</v>
+      </c>
     </row>
-    <row r="40" spans="2:113" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:145" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>89</v>
       </c>
@@ -6532,8 +7709,83 @@
       <c r="DH40" s="2">
         <v>50</v>
       </c>
+      <c r="DI40" s="1">
+        <v>100</v>
+      </c>
+      <c r="DJ40" s="2">
+        <v>50</v>
+      </c>
+      <c r="DK40" s="2">
+        <v>100</v>
+      </c>
+      <c r="DL40" s="1">
+        <v>100</v>
+      </c>
+      <c r="DM40" s="2">
+        <v>100</v>
+      </c>
+      <c r="DN40" s="1">
+        <v>50</v>
+      </c>
+      <c r="DO40" s="2">
+        <v>50</v>
+      </c>
+      <c r="DP40" s="2">
+        <v>50</v>
+      </c>
+      <c r="DQ40" s="2">
+        <v>50</v>
+      </c>
+      <c r="DR40" s="2">
+        <v>100</v>
+      </c>
+      <c r="DT40">
+        <v>50</v>
+      </c>
+      <c r="DU40" s="3">
+        <v>50</v>
+      </c>
+      <c r="DV40" s="3">
+        <v>50</v>
+      </c>
+      <c r="DW40" s="3">
+        <v>50</v>
+      </c>
+      <c r="DY40">
+        <v>50</v>
+      </c>
+      <c r="DZ40">
+        <v>50</v>
+      </c>
+      <c r="EA40" s="11">
+        <v>50</v>
+      </c>
+      <c r="EB40" s="2">
+        <v>100</v>
+      </c>
+      <c r="EC40" s="11">
+        <v>100</v>
+      </c>
+      <c r="EF40">
+        <v>67</v>
+      </c>
+      <c r="EI40">
+        <v>50</v>
+      </c>
+      <c r="EJ40">
+        <v>50</v>
+      </c>
+      <c r="EK40">
+        <v>50</v>
+      </c>
+      <c r="EL40">
+        <v>100</v>
+      </c>
+      <c r="EM40">
+        <v>50</v>
+      </c>
     </row>
-    <row r="41" spans="2:113" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:145" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>90</v>
       </c>
@@ -6784,8 +8036,83 @@
       <c r="DH41" s="2">
         <v>50</v>
       </c>
+      <c r="DI41" s="1">
+        <v>50</v>
+      </c>
+      <c r="DJ41" s="2">
+        <v>50</v>
+      </c>
+      <c r="DK41" s="2">
+        <v>50</v>
+      </c>
+      <c r="DL41" s="1">
+        <v>50</v>
+      </c>
+      <c r="DM41" s="2">
+        <v>50</v>
+      </c>
+      <c r="DN41" s="1">
+        <v>75</v>
+      </c>
+      <c r="DO41" s="2">
+        <v>50</v>
+      </c>
+      <c r="DQ41">
+        <v>50</v>
+      </c>
+      <c r="DS41">
+        <v>50</v>
+      </c>
+      <c r="DT41">
+        <v>50</v>
+      </c>
+      <c r="DU41" s="3">
+        <v>50</v>
+      </c>
+      <c r="DV41" s="3">
+        <v>75</v>
+      </c>
+      <c r="DW41" s="3">
+        <v>50</v>
+      </c>
+      <c r="DX41" s="3">
+        <v>50</v>
+      </c>
+      <c r="DY41" s="3">
+        <v>100</v>
+      </c>
+      <c r="DZ41" s="3">
+        <v>50</v>
+      </c>
+      <c r="EA41" s="11">
+        <v>50</v>
+      </c>
+      <c r="EB41" s="2">
+        <v>75</v>
+      </c>
+      <c r="EC41" s="11">
+        <v>75</v>
+      </c>
+      <c r="EH41">
+        <v>50</v>
+      </c>
+      <c r="EI41">
+        <v>50</v>
+      </c>
+      <c r="EK41">
+        <v>50</v>
+      </c>
+      <c r="EL41">
+        <v>50</v>
+      </c>
+      <c r="EM41">
+        <v>50</v>
+      </c>
+      <c r="EN41">
+        <v>50</v>
+      </c>
     </row>
-    <row r="42" spans="2:113" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:145" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>60</v>
       </c>
@@ -6842,8 +8169,11 @@
       <c r="CZ42" s="2">
         <v>50</v>
       </c>
+      <c r="DY42">
+        <v>50</v>
+      </c>
     </row>
-    <row r="43" spans="2:113" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:145" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>91</v>
       </c>
@@ -7147,8 +8477,83 @@
       <c r="DH43">
         <v>100</v>
       </c>
+      <c r="DI43" s="1">
+        <v>100</v>
+      </c>
+      <c r="DJ43" s="2">
+        <v>100</v>
+      </c>
+      <c r="DK43" s="2">
+        <v>100</v>
+      </c>
+      <c r="DL43" s="1">
+        <v>100</v>
+      </c>
+      <c r="DM43" s="2">
+        <v>100</v>
+      </c>
+      <c r="DN43" s="1">
+        <v>50</v>
+      </c>
+      <c r="DO43" s="2">
+        <v>50</v>
+      </c>
+      <c r="DP43" s="2">
+        <v>50</v>
+      </c>
+      <c r="DQ43" s="2">
+        <v>50</v>
+      </c>
+      <c r="DT43">
+        <v>50</v>
+      </c>
+      <c r="DU43">
+        <v>100</v>
+      </c>
+      <c r="DV43">
+        <v>50</v>
+      </c>
+      <c r="DW43">
+        <v>50</v>
+      </c>
+      <c r="DY43">
+        <v>50</v>
+      </c>
+      <c r="DZ43">
+        <v>50</v>
+      </c>
+      <c r="EA43" s="11">
+        <v>50</v>
+      </c>
+      <c r="EB43" s="2">
+        <v>50</v>
+      </c>
+      <c r="EC43" s="11">
+        <v>100</v>
+      </c>
+      <c r="EH43">
+        <v>50</v>
+      </c>
+      <c r="EI43">
+        <v>50</v>
+      </c>
+      <c r="EK43">
+        <v>100</v>
+      </c>
+      <c r="EL43">
+        <v>100</v>
+      </c>
+      <c r="EM43">
+        <v>50</v>
+      </c>
+      <c r="EN43">
+        <v>50</v>
+      </c>
+      <c r="EO43" s="11">
+        <v>50</v>
+      </c>
     </row>
-    <row r="44" spans="2:113" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:145" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>92</v>
       </c>
@@ -7211,8 +8616,26 @@
       <c r="CY44" s="1">
         <v>100</v>
       </c>
+      <c r="DJ44" s="2">
+        <v>100</v>
+      </c>
+      <c r="DN44" s="1">
+        <v>100</v>
+      </c>
+      <c r="DP44">
+        <v>100</v>
+      </c>
+      <c r="DR44">
+        <v>50</v>
+      </c>
+      <c r="DU44">
+        <v>100</v>
+      </c>
+      <c r="EB44" s="2">
+        <v>100</v>
+      </c>
     </row>
-    <row r="45" spans="2:113" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:145" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>61</v>
       </c>
@@ -7402,8 +8825,80 @@
       <c r="DH45">
         <v>50</v>
       </c>
+      <c r="DI45" s="1">
+        <v>100</v>
+      </c>
+      <c r="DK45">
+        <v>100</v>
+      </c>
+      <c r="DL45" s="1">
+        <v>50</v>
+      </c>
+      <c r="DM45" s="2">
+        <v>50</v>
+      </c>
+      <c r="DP45">
+        <v>50</v>
+      </c>
+      <c r="DQ45">
+        <v>50</v>
+      </c>
+      <c r="DR45">
+        <v>50</v>
+      </c>
+      <c r="DS45">
+        <v>50</v>
+      </c>
+      <c r="DT45">
+        <v>50</v>
+      </c>
+      <c r="DU45">
+        <v>100</v>
+      </c>
+      <c r="DV45">
+        <v>50</v>
+      </c>
+      <c r="DW45">
+        <v>50</v>
+      </c>
+      <c r="DX45">
+        <v>50</v>
+      </c>
+      <c r="DY45">
+        <v>50</v>
+      </c>
+      <c r="DZ45">
+        <v>50</v>
+      </c>
+      <c r="EA45" s="11">
+        <v>50</v>
+      </c>
+      <c r="EB45" s="2">
+        <v>50</v>
+      </c>
+      <c r="EC45" s="11">
+        <v>100</v>
+      </c>
+      <c r="EF45">
+        <v>50</v>
+      </c>
+      <c r="EH45">
+        <v>50</v>
+      </c>
+      <c r="EJ45">
+        <v>50</v>
+      </c>
+      <c r="EK45">
+        <v>50</v>
+      </c>
+      <c r="EM45">
+        <v>50</v>
+      </c>
+      <c r="EO45" s="11">
+        <v>50</v>
+      </c>
     </row>
-    <row r="46" spans="2:113" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:145" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>62</v>
       </c>
@@ -7485,8 +8980,11 @@
       <c r="CW46">
         <v>67</v>
       </c>
+      <c r="DI46" s="1">
+        <v>67</v>
+      </c>
     </row>
-    <row r="47" spans="2:113" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:145" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>93</v>
       </c>
@@ -7596,8 +9094,20 @@
       <c r="DE47">
         <v>100</v>
       </c>
+      <c r="DK47">
+        <v>100</v>
+      </c>
+      <c r="EF47">
+        <v>100</v>
+      </c>
+      <c r="EK47">
+        <v>100</v>
+      </c>
+      <c r="EL47">
+        <v>100</v>
+      </c>
     </row>
-    <row r="48" spans="2:113" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:145" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>63</v>
       </c>
@@ -7738,8 +9248,44 @@
       <c r="DH48">
         <v>50</v>
       </c>
+      <c r="DI48" s="1">
+        <v>50</v>
+      </c>
+      <c r="DJ48" s="2">
+        <v>50</v>
+      </c>
+      <c r="DN48" s="1">
+        <v>50</v>
+      </c>
+      <c r="DV48">
+        <v>50</v>
+      </c>
+      <c r="DY48">
+        <v>50</v>
+      </c>
+      <c r="EH48">
+        <v>50</v>
+      </c>
+      <c r="EI48">
+        <v>50</v>
+      </c>
+      <c r="EJ48">
+        <v>50</v>
+      </c>
+      <c r="EK48">
+        <v>50</v>
+      </c>
+      <c r="EL48">
+        <v>50</v>
+      </c>
+      <c r="EN48">
+        <v>50</v>
+      </c>
+      <c r="EO48" s="11">
+        <v>50</v>
+      </c>
     </row>
-    <row r="49" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:145" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>106</v>
       </c>
@@ -7748,8 +9294,11 @@
       <c r="CY49" s="1">
         <v>100</v>
       </c>
+      <c r="DP49">
+        <v>100</v>
+      </c>
     </row>
-    <row r="50" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:145" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>102</v>
       </c>
@@ -7758,8 +9307,11 @@
       <c r="CF50">
         <v>100</v>
       </c>
+      <c r="DU50">
+        <v>100</v>
+      </c>
     </row>
-    <row r="51" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:145" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>64</v>
       </c>
@@ -7768,8 +9320,11 @@
       </c>
       <c r="G51" s="1"/>
       <c r="X51" s="1"/>
+      <c r="EL51">
+        <v>50</v>
+      </c>
     </row>
-    <row r="52" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:145" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>103</v>
       </c>
@@ -7779,7 +9334,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:145" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>65</v>
       </c>
@@ -7895,8 +9450,17 @@
       <c r="DH53">
         <v>100</v>
       </c>
+      <c r="DI53" s="1">
+        <v>100</v>
+      </c>
+      <c r="EA53" s="11">
+        <v>100</v>
+      </c>
+      <c r="EH53">
+        <v>100</v>
+      </c>
     </row>
-    <row r="54" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:145" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>71</v>
       </c>
@@ -7933,7 +9497,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:145" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>72</v>
       </c>
@@ -7970,408 +9534,527 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:145" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G56" s="1"/>
       <c r="X56" s="1"/>
-      <c r="CC56" s="1">
-        <v>100</v>
-      </c>
-      <c r="CE56">
-        <v>100</v>
-      </c>
-      <c r="CG56">
-        <v>100</v>
-      </c>
-      <c r="CM56">
-        <v>100</v>
-      </c>
-      <c r="CN56">
-        <v>100</v>
-      </c>
-      <c r="CY56" s="1">
+      <c r="DL56" s="1">
+        <v>100</v>
+      </c>
+      <c r="DM56">
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:145" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>66</v>
-      </c>
-      <c r="C57">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="G57" s="1"/>
       <c r="X57" s="1"/>
-      <c r="BF57" s="1">
-        <v>50</v>
-      </c>
-      <c r="BG57">
-        <v>100</v>
-      </c>
-      <c r="BH57">
-        <v>100</v>
-      </c>
-      <c r="BI57">
-        <v>100</v>
-      </c>
-      <c r="BJ57">
-        <v>100</v>
-      </c>
-      <c r="BK57">
-        <v>100</v>
-      </c>
-      <c r="BL57">
-        <v>50</v>
-      </c>
-      <c r="BM57">
-        <v>100</v>
-      </c>
-      <c r="BN57">
-        <v>100</v>
-      </c>
-      <c r="BO57">
-        <v>100</v>
-      </c>
-      <c r="BQ57" s="1">
-        <v>100</v>
-      </c>
-      <c r="BR57" s="2">
-        <v>100</v>
-      </c>
-      <c r="BS57" s="2">
-        <v>50</v>
-      </c>
-      <c r="BT57" s="2">
-        <v>100</v>
-      </c>
-      <c r="BU57" s="2">
-        <v>100</v>
-      </c>
-      <c r="BV57" s="2">
-        <v>100</v>
-      </c>
-      <c r="BW57" s="2">
-        <v>100</v>
-      </c>
-      <c r="BX57" s="2">
-        <v>100</v>
-      </c>
-      <c r="BY57" s="2">
-        <v>50</v>
-      </c>
-      <c r="BZ57" s="2">
-        <v>100</v>
-      </c>
-      <c r="CB57">
-        <v>100</v>
-      </c>
-      <c r="CQ57" s="1">
-        <v>100</v>
-      </c>
-      <c r="CV57">
-        <v>100</v>
-      </c>
-      <c r="CX57">
+      <c r="DL57" s="1">
+        <v>100</v>
+      </c>
+      <c r="DM57">
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:145" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>67</v>
-      </c>
-      <c r="C58">
-        <v>50</v>
-      </c>
-      <c r="D58">
-        <v>50</v>
-      </c>
-      <c r="E58">
-        <v>50</v>
-      </c>
-      <c r="F58">
-        <v>50</v>
-      </c>
-      <c r="G58" s="1">
-        <v>100</v>
-      </c>
-      <c r="H58" s="2">
-        <v>50</v>
-      </c>
-      <c r="I58" s="2">
-        <v>50</v>
-      </c>
-      <c r="J58" s="2">
-        <v>100</v>
-      </c>
-      <c r="K58" s="2">
-        <v>50</v>
-      </c>
-      <c r="M58">
-        <v>100</v>
-      </c>
-      <c r="N58">
-        <v>50</v>
-      </c>
-      <c r="Q58">
-        <v>50</v>
-      </c>
-      <c r="R58">
-        <v>100</v>
-      </c>
-      <c r="T58">
-        <v>50</v>
-      </c>
-      <c r="U58">
-        <v>100</v>
-      </c>
-      <c r="V58">
-        <v>50</v>
-      </c>
-      <c r="X58" s="1">
-        <v>100</v>
-      </c>
-      <c r="Y58" s="2">
-        <v>100</v>
-      </c>
-      <c r="Z58" s="2">
-        <v>100</v>
-      </c>
-      <c r="AA58" s="2">
-        <v>100</v>
-      </c>
-      <c r="AB58" s="2">
-        <v>50</v>
-      </c>
-      <c r="AC58" s="2">
-        <v>100</v>
-      </c>
-      <c r="AD58" s="2">
-        <v>100</v>
-      </c>
-      <c r="AE58" s="2">
-        <v>50</v>
-      </c>
-      <c r="AF58" s="2">
-        <v>100</v>
-      </c>
-      <c r="AG58" s="2">
-        <v>100</v>
-      </c>
-      <c r="AH58" s="2">
-        <v>100</v>
-      </c>
-      <c r="AI58" s="2">
-        <v>100</v>
-      </c>
-      <c r="AJ58" s="2">
-        <v>50</v>
-      </c>
-      <c r="AK58" s="2">
-        <v>100</v>
-      </c>
-      <c r="AM58">
-        <v>100</v>
-      </c>
-      <c r="AO58">
-        <v>50</v>
-      </c>
-      <c r="AP58">
-        <v>50</v>
-      </c>
-      <c r="AQ58">
-        <v>50</v>
-      </c>
-      <c r="AR58">
-        <v>100</v>
-      </c>
-      <c r="AS58">
-        <v>50</v>
-      </c>
-      <c r="AT58">
-        <v>100</v>
-      </c>
-      <c r="AU58">
-        <v>100</v>
-      </c>
-      <c r="AV58">
-        <v>50</v>
-      </c>
-      <c r="AW58">
-        <v>50</v>
-      </c>
-      <c r="AX58">
-        <v>100</v>
-      </c>
-      <c r="AY58">
-        <v>50</v>
-      </c>
-      <c r="AZ58">
-        <v>100</v>
-      </c>
-      <c r="BA58">
-        <v>100</v>
-      </c>
-      <c r="BB58">
-        <v>50</v>
-      </c>
-      <c r="BC58">
-        <v>100</v>
-      </c>
-      <c r="BD58">
-        <v>100</v>
-      </c>
-      <c r="BE58" s="1">
-        <v>100</v>
-      </c>
-      <c r="BF58" s="1">
-        <v>50</v>
-      </c>
-      <c r="BG58" s="2">
-        <v>100</v>
-      </c>
-      <c r="BH58" s="2">
-        <v>100</v>
-      </c>
-      <c r="BJ58">
-        <v>50</v>
-      </c>
-      <c r="BM58">
-        <v>50</v>
-      </c>
-      <c r="BN58">
-        <v>50</v>
-      </c>
-      <c r="BO58">
-        <v>50</v>
-      </c>
-      <c r="BP58">
-        <v>50</v>
-      </c>
-      <c r="BQ58" s="1">
-        <v>50</v>
-      </c>
-      <c r="BR58" s="2">
-        <v>50</v>
-      </c>
-      <c r="BS58" s="2">
-        <v>100</v>
-      </c>
-      <c r="BU58">
-        <v>50</v>
-      </c>
-      <c r="BV58">
-        <v>50</v>
-      </c>
-      <c r="BW58">
-        <v>50</v>
-      </c>
-      <c r="BX58">
-        <v>50</v>
-      </c>
-      <c r="BY58">
-        <v>50</v>
-      </c>
-      <c r="BZ58">
-        <v>100</v>
-      </c>
-      <c r="CA58">
-        <v>50</v>
-      </c>
-      <c r="CB58">
-        <v>50</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="G58" s="1"/>
+      <c r="X58" s="1"/>
       <c r="CC58" s="1">
-        <v>50</v>
-      </c>
-      <c r="CD58" s="2">
-        <v>100</v>
-      </c>
-      <c r="CE58" s="2">
-        <v>100</v>
-      </c>
-      <c r="CF58" s="2">
-        <v>50</v>
-      </c>
-      <c r="CH58">
-        <v>50</v>
-      </c>
-      <c r="CI58">
-        <v>100</v>
-      </c>
-      <c r="CJ58">
-        <v>50</v>
-      </c>
-      <c r="CK58">
-        <v>50</v>
+        <v>100</v>
+      </c>
+      <c r="CE58">
+        <v>100</v>
+      </c>
+      <c r="CG58">
+        <v>100</v>
       </c>
       <c r="CM58">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="CN58">
         <v>100</v>
       </c>
-      <c r="CO58" s="1">
-        <v>50</v>
-      </c>
-      <c r="CP58" s="2">
-        <v>50</v>
-      </c>
-      <c r="CQ58" s="1">
-        <v>100</v>
-      </c>
-      <c r="CR58" s="2">
-        <v>100</v>
-      </c>
-      <c r="CS58" s="2">
-        <v>100</v>
-      </c>
-      <c r="CT58" s="2">
-        <v>100</v>
-      </c>
-      <c r="CV58">
-        <v>100</v>
-      </c>
-      <c r="CW58">
-        <v>50</v>
-      </c>
-      <c r="CX58">
-        <v>50</v>
-      </c>
       <c r="CY58" s="1">
-        <v>50</v>
-      </c>
-      <c r="CZ58" s="2">
-        <v>50</v>
-      </c>
-      <c r="DA58" s="1">
-        <v>100</v>
-      </c>
-      <c r="DB58" s="2">
-        <v>100</v>
-      </c>
-      <c r="DC58" s="2">
-        <v>100</v>
-      </c>
-      <c r="DD58" s="2">
-        <v>100</v>
-      </c>
-      <c r="DE58" s="2">
-        <v>50</v>
-      </c>
-      <c r="DF58" s="2">
-        <v>100</v>
-      </c>
-      <c r="DG58" s="2">
-        <v>50</v>
-      </c>
-      <c r="DH58" s="2">
+        <v>100</v>
+      </c>
+      <c r="DT58">
+        <v>100</v>
+      </c>
+      <c r="DZ58">
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:112" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
+    <row r="59" spans="1:145" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59">
+        <v>100</v>
+      </c>
+      <c r="G59" s="1"/>
+      <c r="X59" s="1"/>
+      <c r="BF59" s="1">
+        <v>50</v>
+      </c>
+      <c r="BG59">
+        <v>100</v>
+      </c>
+      <c r="BH59">
+        <v>100</v>
+      </c>
+      <c r="BI59">
+        <v>100</v>
+      </c>
+      <c r="BJ59">
+        <v>100</v>
+      </c>
+      <c r="BK59">
+        <v>100</v>
+      </c>
+      <c r="BL59">
+        <v>50</v>
+      </c>
+      <c r="BM59">
+        <v>100</v>
+      </c>
+      <c r="BN59">
+        <v>100</v>
+      </c>
+      <c r="BO59">
+        <v>100</v>
+      </c>
+      <c r="BQ59" s="1">
+        <v>100</v>
+      </c>
+      <c r="BR59" s="2">
+        <v>100</v>
+      </c>
+      <c r="BS59" s="2">
+        <v>50</v>
+      </c>
+      <c r="BT59" s="2">
+        <v>100</v>
+      </c>
+      <c r="BU59" s="2">
+        <v>100</v>
+      </c>
+      <c r="BV59" s="2">
+        <v>100</v>
+      </c>
+      <c r="BW59" s="2">
+        <v>100</v>
+      </c>
+      <c r="BX59" s="2">
+        <v>100</v>
+      </c>
+      <c r="BY59" s="2">
+        <v>50</v>
+      </c>
+      <c r="BZ59" s="2">
+        <v>100</v>
+      </c>
+      <c r="CB59">
+        <v>100</v>
+      </c>
+      <c r="CQ59" s="1">
+        <v>100</v>
+      </c>
+      <c r="CV59">
+        <v>100</v>
+      </c>
+      <c r="CX59">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:145" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60">
+        <v>50</v>
+      </c>
+      <c r="D60">
+        <v>50</v>
+      </c>
+      <c r="E60">
+        <v>50</v>
+      </c>
+      <c r="F60">
+        <v>50</v>
+      </c>
+      <c r="G60" s="1">
+        <v>100</v>
+      </c>
+      <c r="H60" s="2">
+        <v>50</v>
+      </c>
+      <c r="I60" s="2">
+        <v>50</v>
+      </c>
+      <c r="J60" s="2">
+        <v>100</v>
+      </c>
+      <c r="K60" s="2">
+        <v>50</v>
+      </c>
+      <c r="M60">
+        <v>100</v>
+      </c>
+      <c r="N60">
+        <v>50</v>
+      </c>
+      <c r="Q60">
+        <v>50</v>
+      </c>
+      <c r="R60">
+        <v>100</v>
+      </c>
+      <c r="T60">
+        <v>50</v>
+      </c>
+      <c r="U60">
+        <v>100</v>
+      </c>
+      <c r="V60">
+        <v>50</v>
+      </c>
+      <c r="X60" s="1">
+        <v>100</v>
+      </c>
+      <c r="Y60" s="2">
+        <v>100</v>
+      </c>
+      <c r="Z60" s="2">
+        <v>100</v>
+      </c>
+      <c r="AA60" s="2">
+        <v>100</v>
+      </c>
+      <c r="AB60" s="2">
+        <v>50</v>
+      </c>
+      <c r="AC60" s="2">
+        <v>100</v>
+      </c>
+      <c r="AD60" s="2">
+        <v>100</v>
+      </c>
+      <c r="AE60" s="2">
+        <v>50</v>
+      </c>
+      <c r="AF60" s="2">
+        <v>100</v>
+      </c>
+      <c r="AG60" s="2">
+        <v>100</v>
+      </c>
+      <c r="AH60" s="2">
+        <v>100</v>
+      </c>
+      <c r="AI60" s="2">
+        <v>100</v>
+      </c>
+      <c r="AJ60" s="2">
+        <v>50</v>
+      </c>
+      <c r="AK60" s="2">
+        <v>100</v>
+      </c>
+      <c r="AM60">
+        <v>100</v>
+      </c>
+      <c r="AO60">
+        <v>50</v>
+      </c>
+      <c r="AP60">
+        <v>50</v>
+      </c>
+      <c r="AQ60">
+        <v>50</v>
+      </c>
+      <c r="AR60">
+        <v>100</v>
+      </c>
+      <c r="AS60">
+        <v>50</v>
+      </c>
+      <c r="AT60">
+        <v>100</v>
+      </c>
+      <c r="AU60">
+        <v>100</v>
+      </c>
+      <c r="AV60">
+        <v>50</v>
+      </c>
+      <c r="AW60">
+        <v>50</v>
+      </c>
+      <c r="AX60">
+        <v>100</v>
+      </c>
+      <c r="AY60">
+        <v>50</v>
+      </c>
+      <c r="AZ60">
+        <v>100</v>
+      </c>
+      <c r="BA60">
+        <v>100</v>
+      </c>
+      <c r="BB60">
+        <v>50</v>
+      </c>
+      <c r="BC60">
+        <v>100</v>
+      </c>
+      <c r="BD60">
+        <v>100</v>
+      </c>
+      <c r="BE60" s="1">
+        <v>100</v>
+      </c>
+      <c r="BF60" s="1">
+        <v>50</v>
+      </c>
+      <c r="BG60" s="2">
+        <v>100</v>
+      </c>
+      <c r="BH60" s="2">
+        <v>100</v>
+      </c>
+      <c r="BJ60">
+        <v>50</v>
+      </c>
+      <c r="BM60">
+        <v>50</v>
+      </c>
+      <c r="BN60">
+        <v>50</v>
+      </c>
+      <c r="BO60">
+        <v>50</v>
+      </c>
+      <c r="BP60">
+        <v>50</v>
+      </c>
+      <c r="BQ60" s="1">
+        <v>50</v>
+      </c>
+      <c r="BR60" s="2">
+        <v>50</v>
+      </c>
+      <c r="BS60" s="2">
+        <v>100</v>
+      </c>
+      <c r="BU60">
+        <v>50</v>
+      </c>
+      <c r="BV60">
+        <v>50</v>
+      </c>
+      <c r="BW60">
+        <v>50</v>
+      </c>
+      <c r="BX60">
+        <v>50</v>
+      </c>
+      <c r="BY60">
+        <v>50</v>
+      </c>
+      <c r="BZ60">
+        <v>100</v>
+      </c>
+      <c r="CA60">
+        <v>50</v>
+      </c>
+      <c r="CB60">
+        <v>50</v>
+      </c>
+      <c r="CC60" s="1">
+        <v>50</v>
+      </c>
+      <c r="CD60" s="2">
+        <v>100</v>
+      </c>
+      <c r="CE60" s="2">
+        <v>100</v>
+      </c>
+      <c r="CF60" s="2">
+        <v>50</v>
+      </c>
+      <c r="CH60">
+        <v>50</v>
+      </c>
+      <c r="CI60">
+        <v>100</v>
+      </c>
+      <c r="CJ60">
+        <v>50</v>
+      </c>
+      <c r="CK60">
+        <v>50</v>
+      </c>
+      <c r="CM60">
+        <v>50</v>
+      </c>
+      <c r="CN60">
+        <v>100</v>
+      </c>
+      <c r="CO60" s="1">
+        <v>50</v>
+      </c>
+      <c r="CP60" s="2">
+        <v>50</v>
+      </c>
+      <c r="CQ60" s="1">
+        <v>100</v>
+      </c>
+      <c r="CR60" s="2">
+        <v>100</v>
+      </c>
+      <c r="CS60" s="2">
+        <v>100</v>
+      </c>
+      <c r="CT60" s="2">
+        <v>100</v>
+      </c>
+      <c r="CV60">
+        <v>100</v>
+      </c>
+      <c r="CW60">
+        <v>50</v>
+      </c>
+      <c r="CX60">
+        <v>50</v>
+      </c>
+      <c r="CY60" s="1">
+        <v>50</v>
+      </c>
+      <c r="CZ60" s="2">
+        <v>50</v>
+      </c>
+      <c r="DA60" s="1">
+        <v>100</v>
+      </c>
+      <c r="DB60" s="2">
+        <v>100</v>
+      </c>
+      <c r="DC60" s="2">
+        <v>100</v>
+      </c>
+      <c r="DD60" s="2">
+        <v>100</v>
+      </c>
+      <c r="DE60" s="2">
+        <v>50</v>
+      </c>
+      <c r="DF60" s="2">
+        <v>100</v>
+      </c>
+      <c r="DG60" s="2">
+        <v>50</v>
+      </c>
+      <c r="DH60" s="2">
+        <v>100</v>
+      </c>
+      <c r="DI60" s="1">
+        <v>100</v>
+      </c>
+      <c r="DJ60" s="2">
+        <v>50</v>
+      </c>
+      <c r="DK60" s="2">
+        <v>50</v>
+      </c>
+      <c r="DL60" s="1">
+        <v>100</v>
+      </c>
+      <c r="DM60" s="2">
+        <v>50</v>
+      </c>
+      <c r="DN60" s="1">
+        <v>50</v>
+      </c>
+      <c r="DO60" s="2">
+        <v>100</v>
+      </c>
+      <c r="DP60" s="2">
+        <v>100</v>
+      </c>
+      <c r="DQ60" s="2">
+        <v>50</v>
+      </c>
+      <c r="DS60">
+        <v>50</v>
+      </c>
+      <c r="DT60">
+        <v>50</v>
+      </c>
+      <c r="DU60">
+        <v>50</v>
+      </c>
+      <c r="DV60">
+        <v>100</v>
+      </c>
+      <c r="DX60">
+        <v>50</v>
+      </c>
+      <c r="DY60">
+        <v>50</v>
+      </c>
+      <c r="EA60" s="11">
+        <v>100</v>
+      </c>
+      <c r="EB60" s="2">
+        <v>100</v>
+      </c>
+      <c r="EC60" s="11">
+        <v>50</v>
+      </c>
+      <c r="EE60">
+        <v>50</v>
+      </c>
+      <c r="EF60">
+        <v>50</v>
+      </c>
+      <c r="EG60" s="11">
+        <v>50</v>
+      </c>
+      <c r="EH60" s="2">
+        <v>100</v>
+      </c>
+      <c r="EI60" s="2">
+        <v>100</v>
+      </c>
+      <c r="EJ60" s="2">
+        <v>100</v>
+      </c>
+      <c r="EK60" s="2">
+        <v>100</v>
+      </c>
+      <c r="EL60" s="2">
+        <v>50</v>
+      </c>
+      <c r="EM60" s="2">
+        <v>100</v>
+      </c>
+      <c r="EN60" s="2">
+        <v>50</v>
+      </c>
+      <c r="EO60" s="11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:145" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add methonal degraders to consolidated pathway.
</commit_message>
<xml_diff>
--- a/Pathway_analysis/consolidated_pathway_data.xlsx
+++ b/Pathway_analysis/consolidated_pathway_data.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Desktop\MAGstravaganza\Pathway_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amlin\Desktop\MAGstravaganza\Pathway_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{E939C158-CBE7-4350-A3D4-5E6F520EE9A7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -362,7 +362,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -792,14 +792,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60D4974-3795-4306-8C06-8E8279D3D854}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GN65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="FX3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="FU3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="GJ12" sqref="GJ11:GJ12"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,6 +2504,9 @@
       <c r="B7" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="C7" s="3">
+        <v>100</v>
+      </c>
       <c r="G7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="2"/>
@@ -2520,7 +2523,9 @@
       <c r="CE7" s="2"/>
       <c r="CF7" s="2"/>
       <c r="CG7" s="2"/>
-      <c r="CH7" s="2"/>
+      <c r="CH7" s="2">
+        <v>100</v>
+      </c>
       <c r="CI7" s="2">
         <v>100</v>
       </c>
@@ -2534,7 +2539,21 @@
       <c r="DA7" s="4"/>
       <c r="DI7" s="4"/>
       <c r="DL7" s="4"/>
-      <c r="DN7" s="4"/>
+      <c r="DN7" s="4">
+        <v>100</v>
+      </c>
+      <c r="DQ7" s="3">
+        <v>100</v>
+      </c>
+      <c r="DV7" s="3">
+        <v>100</v>
+      </c>
+      <c r="DY7" s="3">
+        <v>100</v>
+      </c>
+      <c r="DZ7" s="3">
+        <v>100</v>
+      </c>
       <c r="EA7" s="10"/>
       <c r="EC7" s="10"/>
       <c r="EG7" s="10"/>
@@ -2543,7 +2562,36 @@
       <c r="FA7" s="10"/>
       <c r="FC7" s="10"/>
       <c r="FE7" s="10"/>
-      <c r="GF7" s="10"/>
+      <c r="FI7" s="3">
+        <v>100</v>
+      </c>
+      <c r="FK7" s="3">
+        <v>100</v>
+      </c>
+      <c r="FU7" s="3">
+        <v>100</v>
+      </c>
+      <c r="FW7" s="3">
+        <v>100</v>
+      </c>
+      <c r="FX7" s="3">
+        <v>100</v>
+      </c>
+      <c r="FZ7" s="3">
+        <v>100</v>
+      </c>
+      <c r="GA7" s="3">
+        <v>100</v>
+      </c>
+      <c r="GC7" s="3">
+        <v>100</v>
+      </c>
+      <c r="GE7" s="3">
+        <v>100</v>
+      </c>
+      <c r="GF7" s="10">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="2:196" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">

</xml_diff>